<commit_message>
Figured out quality steps making inroads with traffic light from scratch in qualinprogress.R adding quality toggle to quality_scores_vals fleshing out SR rmd
</commit_message>
<xml_diff>
--- a/quality_scores.xlsx
+++ b/quality_scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/2509920f_student_gla_ac_uk/Documents/DClin/Deliverables/Systematic Review/Writeup/DCLIN_SR_git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_D3E6F2390019EBBA504521FA5F3D01F7BA1BD057" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0CD7EC0-645B-40C6-B3D5-51E516BEB90E}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="11_D3E6F2390019EBBA504521FA5F3D01F7BA1BD057" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{329C4B9A-2C32-40C9-9B45-16509BCE9104}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="127">
   <si>
     <t>Study</t>
   </si>
@@ -197,6 +197,210 @@
   </si>
   <si>
     <t>MED128</t>
+  </si>
+  <si>
+    <t>Weiner et al. (2006)</t>
+  </si>
+  <si>
+    <t>Al-Malki et al. (2020)</t>
+  </si>
+  <si>
+    <t>Cardoso et al. (2021)</t>
+  </si>
+  <si>
+    <t>Barceló-Martinez et al. (2018)</t>
+  </si>
+  <si>
+    <t>Boldt et al. (2020)</t>
+  </si>
+  <si>
+    <t>Borg et al. (2015)</t>
+  </si>
+  <si>
+    <t>Buckalew et al. (2008)</t>
+  </si>
+  <si>
+    <t>Can et al. (2012)</t>
+  </si>
+  <si>
+    <t>Chen et al. (2017)</t>
+  </si>
+  <si>
+    <t>Chen et al. (2016)</t>
+  </si>
+  <si>
+    <t>CHE063-A</t>
+  </si>
+  <si>
+    <t>Coelho Rebelo Maia (2012)</t>
+  </si>
+  <si>
+    <t>Corti et al. (2021)</t>
+  </si>
+  <si>
+    <t>Demirci &amp; Savas (2002)</t>
+  </si>
+  <si>
+    <t>Di Carlo et al. (2021)</t>
+  </si>
+  <si>
+    <t>El-Shafey et al. (2012)</t>
+  </si>
+  <si>
+    <t>Fayed et al. (2012)</t>
+  </si>
+  <si>
+    <t>FAY089-A</t>
+  </si>
+  <si>
+    <t>Fayed et al. (2017)</t>
+  </si>
+  <si>
+    <t>Feng et al. (2020)</t>
+  </si>
+  <si>
+    <t>Foss et al. (2016)</t>
+  </si>
+  <si>
+    <t>Garcia et al. (2021)</t>
+  </si>
+  <si>
+    <t>Gwinnutt et al. (2021)</t>
+  </si>
+  <si>
+    <t>Karp et al. (2008)</t>
+  </si>
+  <si>
+    <t>Kim &amp; Buschmann (2006)</t>
+  </si>
+  <si>
+    <t>Li et al. (2018)</t>
+  </si>
+  <si>
+    <t>Liao et al. (2018)</t>
+  </si>
+  <si>
+    <t>LIA121-A</t>
+  </si>
+  <si>
+    <t>Ma et al. (2017)</t>
+  </si>
+  <si>
+    <t>Ojeda et al. (2016)</t>
+  </si>
+  <si>
+    <t>OJE134-NP-A</t>
+  </si>
+  <si>
+    <t>Oláh et al. (2020)</t>
+  </si>
+  <si>
+    <t>Oosterman et al. (2011)</t>
+  </si>
+  <si>
+    <t>Petersen et al. (2015)</t>
+  </si>
+  <si>
+    <t>Qu et al. (2018)</t>
+  </si>
+  <si>
+    <t>Ruscheweyh et al. (2018)</t>
+  </si>
+  <si>
+    <t>Seo et al. (2017)</t>
+  </si>
+  <si>
+    <t>Shehata et al. (2010)</t>
+  </si>
+  <si>
+    <t>Terassi et al. (2021)</t>
+  </si>
+  <si>
+    <t>TER167-COMB</t>
+  </si>
+  <si>
+    <t>Tiwari et al. (2021)</t>
+  </si>
+  <si>
+    <t>Torkamani et al. (2015)</t>
+  </si>
+  <si>
+    <t>Veldhuijzen et al. (2012)</t>
+  </si>
+  <si>
+    <t>R. Wang et al. (2014)</t>
+  </si>
+  <si>
+    <t>WAN182-A</t>
+  </si>
+  <si>
+    <t>Y. Wang et al. (2014)</t>
+  </si>
+  <si>
+    <t>Canfora et al. (2021)</t>
+  </si>
+  <si>
+    <t>Segura-Jiménez et al. (2015)</t>
+  </si>
+  <si>
+    <t>Mednieks et al. (2021)</t>
+  </si>
+  <si>
+    <t>Xiang et al. (2021)</t>
+  </si>
+  <si>
+    <t>XIA186</t>
+  </si>
+  <si>
+    <t>Maneeton et al. (2010)</t>
+  </si>
+  <si>
+    <t>MAN998</t>
+  </si>
+  <si>
+    <t>Hamed et al. (2012)</t>
+  </si>
+  <si>
+    <t>HAM196</t>
+  </si>
+  <si>
+    <t>Baptista et al. (2017)</t>
+  </si>
+  <si>
+    <t>BAP992</t>
+  </si>
+  <si>
+    <t>Vitturi et al. (2019)</t>
+  </si>
+  <si>
+    <t>VIT197-A</t>
+  </si>
+  <si>
+    <t>VIT197-B</t>
+  </si>
+  <si>
+    <t>Peterson et al. (2018)</t>
+  </si>
+  <si>
+    <t>PET994-A</t>
+  </si>
+  <si>
+    <t>Güzel et al. (2018)</t>
+  </si>
+  <si>
+    <t>GUZ995</t>
+  </si>
+  <si>
+    <t>Kotb et al. (2019)</t>
+  </si>
+  <si>
+    <t>KOT997</t>
+  </si>
+  <si>
+    <t>Petra et al. (2020)</t>
+  </si>
+  <si>
+    <t>PET991</t>
   </si>
 </sst>
 </file>
@@ -238,7 +442,38 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -530,15 +765,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -570,7 +805,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -601,8 +836,14 @@
       <c r="J2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -633,8 +874,14 @@
       <c r="J3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -665,8 +912,14 @@
       <c r="J4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -697,8 +950,14 @@
       <c r="J5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -729,8 +988,14 @@
       <c r="J6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>63</v>
+      </c>
+      <c r="L6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -761,8 +1026,14 @@
       <c r="J7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>64</v>
+      </c>
+      <c r="L7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -793,8 +1064,14 @@
       <c r="J8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>65</v>
+      </c>
+      <c r="L8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -825,8 +1102,14 @@
       <c r="J9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>66</v>
+      </c>
+      <c r="L9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -857,8 +1140,14 @@
       <c r="J10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>67</v>
+      </c>
+      <c r="L10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -889,8 +1178,14 @@
       <c r="J11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>68</v>
+      </c>
+      <c r="L11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -921,8 +1216,14 @@
       <c r="J12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" t="s">
+        <v>70</v>
+      </c>
+      <c r="L12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -953,8 +1254,14 @@
       <c r="J13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>71</v>
+      </c>
+      <c r="L13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -985,8 +1292,14 @@
       <c r="J14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
+        <v>72</v>
+      </c>
+      <c r="L14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1017,8 +1330,14 @@
       <c r="J15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>73</v>
+      </c>
+      <c r="L15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1049,8 +1368,14 @@
       <c r="J16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>74</v>
+      </c>
+      <c r="L16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1081,8 +1406,14 @@
       <c r="J17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>75</v>
+      </c>
+      <c r="L17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -1113,8 +1444,14 @@
       <c r="J18" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>77</v>
+      </c>
+      <c r="L18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1145,8 +1482,14 @@
       <c r="J19" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" t="s">
+        <v>78</v>
+      </c>
+      <c r="L19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -1177,8 +1520,14 @@
       <c r="J20" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" t="s">
+        <v>79</v>
+      </c>
+      <c r="L20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -1209,8 +1558,14 @@
       <c r="J21" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" t="s">
+        <v>80</v>
+      </c>
+      <c r="L21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -1241,8 +1596,14 @@
       <c r="J22" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" t="s">
+        <v>81</v>
+      </c>
+      <c r="L22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1273,8 +1634,14 @@
       <c r="J23" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>82</v>
+      </c>
+      <c r="L23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -1305,8 +1672,14 @@
       <c r="J24" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" t="s">
+        <v>83</v>
+      </c>
+      <c r="L24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -1337,8 +1710,14 @@
       <c r="J25" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
+        <v>84</v>
+      </c>
+      <c r="L25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1369,8 +1748,14 @@
       <c r="J26" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" t="s">
+        <v>85</v>
+      </c>
+      <c r="L26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -1401,8 +1786,14 @@
       <c r="J27" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27" t="s">
+        <v>87</v>
+      </c>
+      <c r="L27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -1433,8 +1824,14 @@
       <c r="J28" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" t="s">
+        <v>88</v>
+      </c>
+      <c r="L28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -1465,8 +1862,14 @@
       <c r="J29" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29" t="s">
+        <v>90</v>
+      </c>
+      <c r="L29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -1497,8 +1900,14 @@
       <c r="J30" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30" t="s">
+        <v>91</v>
+      </c>
+      <c r="L30" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>44</v>
       </c>
@@ -1529,8 +1938,14 @@
       <c r="J31" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
+        <v>92</v>
+      </c>
+      <c r="L31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -1561,8 +1976,14 @@
       <c r="J32" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K32" t="s">
+        <v>93</v>
+      </c>
+      <c r="L32" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>46</v>
       </c>
@@ -1593,8 +2014,14 @@
       <c r="J33" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33" t="s">
+        <v>94</v>
+      </c>
+      <c r="L33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>47</v>
       </c>
@@ -1625,8 +2052,14 @@
       <c r="J34" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K34" t="s">
+        <v>95</v>
+      </c>
+      <c r="L34" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -1657,8 +2090,14 @@
       <c r="J35" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K35" t="s">
+        <v>96</v>
+      </c>
+      <c r="L35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>49</v>
       </c>
@@ -1689,8 +2128,14 @@
       <c r="J36" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K36" t="s">
+        <v>97</v>
+      </c>
+      <c r="L36" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>50</v>
       </c>
@@ -1721,8 +2166,14 @@
       <c r="J37" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K37" t="s">
+        <v>99</v>
+      </c>
+      <c r="L37" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>51</v>
       </c>
@@ -1753,8 +2204,14 @@
       <c r="J38" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K38" t="s">
+        <v>100</v>
+      </c>
+      <c r="L38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -1785,8 +2242,14 @@
       <c r="J39" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K39" t="s">
+        <v>101</v>
+      </c>
+      <c r="L39" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>53</v>
       </c>
@@ -1817,8 +2280,14 @@
       <c r="J40" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K40" t="s">
+        <v>102</v>
+      </c>
+      <c r="L40" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -1849,8 +2318,14 @@
       <c r="J41" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K41" t="s">
+        <v>104</v>
+      </c>
+      <c r="L41" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>55</v>
       </c>
@@ -1881,8 +2356,14 @@
       <c r="J42" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K42" t="s">
+        <v>105</v>
+      </c>
+      <c r="L42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>56</v>
       </c>
@@ -1913,8 +2394,14 @@
       <c r="J43" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K43" t="s">
+        <v>106</v>
+      </c>
+      <c r="L43" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>57</v>
       </c>
@@ -1945,8 +2432,14 @@
       <c r="J44" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K44" t="s">
+        <v>107</v>
+      </c>
+      <c r="L44" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -1977,8 +2470,94 @@
       <c r="J45" t="s">
         <v>14</v>
       </c>
+      <c r="K45" t="s">
+        <v>108</v>
+      </c>
+      <c r="L45" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K46" t="s">
+        <v>110</v>
+      </c>
+      <c r="L46" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K47" t="s">
+        <v>112</v>
+      </c>
+      <c r="L47" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K48" t="s">
+        <v>114</v>
+      </c>
+      <c r="L48" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K49" t="s">
+        <v>116</v>
+      </c>
+      <c r="L49" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K50" t="s">
+        <v>116</v>
+      </c>
+      <c r="L50" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="51" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K51" t="s">
+        <v>119</v>
+      </c>
+      <c r="L51" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="52" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K52" t="s">
+        <v>121</v>
+      </c>
+      <c r="L52" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="53" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K53" t="s">
+        <v>123</v>
+      </c>
+      <c r="L53" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="54" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K54" t="s">
+        <v>125</v>
+      </c>
+      <c r="L54" t="s">
+        <v>126</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:H45">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>